<commit_message>
Datos modificados y nuevos archivos para graficar
</commit_message>
<xml_diff>
--- a/Código PAPER/modelo/data/input/datos_finales30.xlsx
+++ b/Código PAPER/modelo/data/input/datos_finales30.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camilomerino/Documents/IPre/IEE2985-2/Código PAPER/modelo/data/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ff7811548ae3acaf/Documentos/GitHub/IEE2985/Código PAPER/modelo/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980BB2A6-2B7B-574E-91E4-3A6BED000D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{980BB2A6-2B7B-574E-91E4-3A6BED000D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA45E218-A98C-4EAD-9062-363AE6CA536C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="31400" windowHeight="17100" xr2:uid="{80E02269-A3DD-48C4-A8B7-66D9192E8AAD}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{80E02269-A3DD-48C4-A8B7-66D9192E8AAD}"/>
   </bookViews>
   <sheets>
     <sheet name="BUS DATA" sheetId="1" r:id="rId1"/>
@@ -260,6 +260,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -302,11 +305,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -322,6 +326,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -643,17 +651,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C404ACF8-4AE1-492F-B81B-865E1642AE83}">
   <dimension ref="A1:AL67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2:AL31"/>
+    <sheetView tabSelected="1" topLeftCell="H16" workbookViewId="0">
+      <selection activeCell="O34" sqref="O34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6328125" customWidth="1"/>
+    <col min="10" max="10" width="13.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -769,7 +777,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -788,9 +796,7 @@
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
-      <c r="M2" s="3">
-        <v>1</v>
-      </c>
+      <c r="M2" s="4"/>
       <c r="N2" s="3">
         <v>2</v>
       </c>
@@ -867,7 +873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -904,8 +910,8 @@
       <c r="L3" s="3">
         <v>3</v>
       </c>
-      <c r="M3" s="3">
-        <v>5</v>
+      <c r="M3" s="4">
+        <v>5.165</v>
       </c>
       <c r="N3" s="3">
         <v>0.2</v>
@@ -983,7 +989,7 @@
         <v>99.675385000000006</v>
       </c>
     </row>
-    <row r="4" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1020,8 +1026,8 @@
       <c r="L4" s="3">
         <v>3</v>
       </c>
-      <c r="M4" s="3">
-        <v>5</v>
+      <c r="M4" s="4">
+        <v>5.165</v>
       </c>
       <c r="N4" s="3">
         <v>0.22</v>
@@ -1099,7 +1105,7 @@
         <v>1.9935080000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1136,8 +1142,8 @@
       <c r="L5" s="3">
         <v>2</v>
       </c>
-      <c r="M5" s="3">
-        <v>5</v>
+      <c r="M5" s="4">
+        <v>5.165</v>
       </c>
       <c r="N5" s="3">
         <v>0.25</v>
@@ -1215,7 +1221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1252,8 +1258,8 @@
       <c r="L6" s="3">
         <v>1</v>
       </c>
-      <c r="M6" s="3">
-        <v>5</v>
+      <c r="M6" s="4">
+        <v>5.165</v>
       </c>
       <c r="N6" s="3">
         <v>0.27</v>
@@ -1331,7 +1337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1350,7 +1356,7 @@
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
+      <c r="M7" s="4"/>
       <c r="N7" s="3"/>
       <c r="O7">
         <v>0</v>
@@ -1425,7 +1431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1444,7 +1450,7 @@
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
+      <c r="M8" s="4"/>
       <c r="N8" s="3"/>
       <c r="O8">
         <v>21.226111</v>
@@ -1519,7 +1525,7 @@
         <v>23.216058</v>
       </c>
     </row>
-    <row r="9" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1538,7 +1544,7 @@
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
+      <c r="M9" s="4"/>
       <c r="N9" s="3"/>
       <c r="O9">
         <v>0</v>
@@ -1613,7 +1619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1632,7 +1638,7 @@
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
+      <c r="M10" s="4"/>
       <c r="N10" s="3"/>
       <c r="O10">
         <v>0</v>
@@ -1707,7 +1713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1726,7 +1732,7 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
+      <c r="M11" s="4"/>
       <c r="N11" s="3"/>
       <c r="O11">
         <v>5.7716789999999998</v>
@@ -1801,7 +1807,7 @@
         <v>6.3127740000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1820,7 +1826,7 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
+      <c r="M12" s="4"/>
       <c r="N12" s="3"/>
       <c r="O12">
         <v>0</v>
@@ -1895,7 +1901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1914,7 +1920,7 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
+      <c r="M13" s="4"/>
       <c r="N13" s="3"/>
       <c r="O13">
         <v>10.859870000000001</v>
@@ -1989,7 +1995,7 @@
         <v>11.877983</v>
       </c>
     </row>
-    <row r="14" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2008,7 +2014,7 @@
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
+      <c r="M14" s="4"/>
       <c r="N14" s="3"/>
       <c r="O14">
         <v>0</v>
@@ -2083,7 +2089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2102,7 +2108,7 @@
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
+      <c r="M15" s="4"/>
       <c r="N15" s="3"/>
       <c r="O15">
         <v>5.8855940000000002</v>
@@ -2177,7 +2183,7 @@
         <v>6.4373690000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2196,7 +2202,7 @@
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
+      <c r="M16" s="4"/>
       <c r="N16" s="3"/>
       <c r="O16">
         <v>7.8980880000000004</v>
@@ -2271,7 +2277,7 @@
         <v>8.6385330000000007</v>
       </c>
     </row>
-    <row r="17" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2290,7 +2296,7 @@
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
+      <c r="M17" s="4"/>
       <c r="N17" s="3"/>
       <c r="O17">
         <v>3.5313560000000002</v>
@@ -2365,7 +2371,7 @@
         <v>3.8624209999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2384,7 +2390,7 @@
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
+      <c r="M18" s="4"/>
       <c r="N18" s="3"/>
       <c r="O18">
         <v>8.8094049999999999</v>
@@ -2459,7 +2465,7 @@
         <v>9.6352869999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2478,7 +2484,7 @@
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
       <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
+      <c r="M19" s="4"/>
       <c r="N19" s="3"/>
       <c r="O19">
         <v>3.2275839999999998</v>
@@ -2553,7 +2559,7 @@
         <v>3.53017</v>
       </c>
     </row>
-    <row r="20" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2572,7 +2578,7 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
+      <c r="M20" s="4"/>
       <c r="N20" s="3"/>
       <c r="O20">
         <v>8.8094049999999999</v>
@@ -2647,7 +2653,7 @@
         <v>9.6352869999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2666,7 +2672,7 @@
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
       <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
+      <c r="M21" s="4"/>
       <c r="N21" s="3"/>
       <c r="O21">
         <v>2.0884369999999999</v>
@@ -2741,7 +2747,7 @@
         <v>2.2842280000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2760,7 +2766,7 @@
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
       <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
+      <c r="M22" s="4"/>
       <c r="N22" s="3"/>
       <c r="O22">
         <v>17.163152</v>
@@ -2835,7 +2841,7 @@
         <v>18.772196999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2854,7 +2860,7 @@
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
+      <c r="M23" s="4"/>
       <c r="N23" s="3"/>
       <c r="O23">
         <v>0</v>
@@ -2929,7 +2935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -2948,9 +2954,7 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
-      <c r="M24" s="3">
-        <v>1</v>
-      </c>
+      <c r="M24" s="4"/>
       <c r="N24" s="3">
         <v>2</v>
       </c>
@@ -3027,7 +3031,7 @@
         <v>3.53017</v>
       </c>
     </row>
-    <row r="25" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -3046,7 +3050,7 @@
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
+      <c r="M25" s="4"/>
       <c r="N25" s="3"/>
       <c r="O25">
         <v>7.9740310000000001</v>
@@ -3121,7 +3125,7 @@
         <v>8.7215959999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -3140,7 +3144,7 @@
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
+      <c r="M26" s="4"/>
       <c r="N26" s="3"/>
       <c r="O26">
         <v>0</v>
@@ -3215,7 +3219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:38" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -3234,9 +3238,7 @@
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
-      <c r="M27" s="3">
-        <v>1</v>
-      </c>
+      <c r="M27" s="4"/>
       <c r="N27" s="3">
         <v>2</v>
       </c>
@@ -3313,7 +3315,7 @@
         <v>3.8624209999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:38" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -3350,8 +3352,8 @@
       <c r="L28" s="3">
         <v>2</v>
       </c>
-      <c r="M28" s="3">
-        <v>5</v>
+      <c r="M28" s="4">
+        <v>5.165</v>
       </c>
       <c r="N28" s="3">
         <v>0.26</v>
@@ -3429,7 +3431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:38" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -3448,7 +3450,7 @@
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
+      <c r="M29" s="4"/>
       <c r="N29" s="3"/>
       <c r="O29">
         <v>0</v>
@@ -3523,7 +3525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:38" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -3542,7 +3544,7 @@
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
+      <c r="M30" s="4"/>
       <c r="N30" s="3"/>
       <c r="O30">
         <v>2.278295</v>
@@ -3617,7 +3619,7 @@
         <v>2.4918849999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:38" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -3654,8 +3656,8 @@
       <c r="L31" s="3">
         <v>1</v>
       </c>
-      <c r="M31" s="3">
-        <v>5</v>
+      <c r="M31" s="4">
+        <v>5.165</v>
       </c>
       <c r="N31" s="3">
         <v>0.28000000000000003</v>
@@ -3733,40 +3735,40 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:38" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="6:6" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:38" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="6:6" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="38" spans="6:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F38" s="2"/>
     </row>
-    <row r="39" spans="6:6" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="6:6" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="6:6" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="6:6" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="6:6" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="6:6" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="6:6" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="6:6" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="6:6" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="6:6" x14ac:dyDescent="0.2"/>
-    <row r="49" x14ac:dyDescent="0.2"/>
-    <row r="50" x14ac:dyDescent="0.2"/>
-    <row r="51" x14ac:dyDescent="0.2"/>
-    <row r="52" x14ac:dyDescent="0.2"/>
-    <row r="53" x14ac:dyDescent="0.2"/>
-    <row r="54" x14ac:dyDescent="0.2"/>
-    <row r="55" x14ac:dyDescent="0.2"/>
-    <row r="56" x14ac:dyDescent="0.2"/>
-    <row r="57" x14ac:dyDescent="0.2"/>
-    <row r="58" x14ac:dyDescent="0.2"/>
-    <row r="59" x14ac:dyDescent="0.2"/>
-    <row r="60" x14ac:dyDescent="0.2"/>
-    <row r="61" x14ac:dyDescent="0.2"/>
-    <row r="62" x14ac:dyDescent="0.2"/>
-    <row r="63" x14ac:dyDescent="0.2"/>
-    <row r="64" x14ac:dyDescent="0.2"/>
-    <row r="65" x14ac:dyDescent="0.2"/>
-    <row r="66" x14ac:dyDescent="0.2"/>
-    <row r="67" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="6:6" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="40" spans="6:6" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="41" spans="6:6" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="42" spans="6:6" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="43" spans="6:6" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="44" spans="6:6" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="45" spans="6:6" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="46" spans="6:6" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="47" spans="6:6" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="48" spans="6:6" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="49" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="50" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="51" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="52" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="53" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="54" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="55" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="56" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="57" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="58" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="59" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="60" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="61" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="62" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="63" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="64" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="65" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="66" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="67" ht="14.5" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3781,9 +3783,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>0</v>
       </c>
@@ -3857,7 +3859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3931,7 +3933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1.488</v>
       </c>
@@ -4005,7 +4007,7 @@
         <v>1.488</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>4.7119999999999997</v>
       </c>
@@ -4079,7 +4081,7 @@
         <v>4.7119999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>0</v>
       </c>
@@ -4153,7 +4155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>0</v>
       </c>
@@ -4227,7 +4229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>14.135999999999999</v>
       </c>
@@ -4301,7 +4303,7 @@
         <v>14.135999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>0</v>
       </c>
@@ -4375,7 +4377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>0</v>
       </c>
@@ -4449,7 +4451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>3.5960000000000001</v>
       </c>
@@ -4523,7 +4525,7 @@
         <v>3.5960000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>0</v>
       </c>
@@ -4591,7 +4593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>6.944</v>
       </c>
@@ -4665,7 +4667,7 @@
         <v>6.944</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>0</v>
       </c>
@@ -4733,7 +4735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>3.8439999999999999</v>
       </c>
@@ -4807,7 +4809,7 @@
         <v>3.8439999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>5.0839999999999996</v>
       </c>
@@ -4881,7 +4883,7 @@
         <v>5.0839999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2.17</v>
       </c>
@@ -4955,7 +4957,7 @@
         <v>2.17</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>5.58</v>
       </c>
@@ -5029,7 +5031,7 @@
         <v>5.58</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>1.984</v>
       </c>
@@ -5103,7 +5105,7 @@
         <v>1.984</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>5.89</v>
       </c>
@@ -5177,7 +5179,7 @@
         <v>5.89</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1.3640000000000001</v>
       </c>
@@ -5251,7 +5253,7 @@
         <v>1.3640000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>10.85</v>
       </c>
@@ -5325,7 +5327,7 @@
         <v>10.85</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>0</v>
       </c>
@@ -5399,7 +5401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>1.984</v>
       </c>
@@ -5473,7 +5475,7 @@
         <v>1.984</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>5.3940000000000001</v>
       </c>
@@ -5547,7 +5549,7 @@
         <v>5.3940000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>0</v>
       </c>
@@ -5621,7 +5623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2.17</v>
       </c>
@@ -5695,7 +5697,7 @@
         <v>2.17</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>0</v>
       </c>
@@ -5769,7 +5771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>0</v>
       </c>
@@ -5843,7 +5845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>1.488</v>
       </c>
@@ -5917,7 +5919,7 @@
         <v>1.488</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>6.5720000000000001</v>
       </c>
@@ -5991,7 +5993,7 @@
         <v>6.5720000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A31">
         <f>SUM(A1:A30)</f>
         <v>85.25</v>
@@ -6102,12 +6104,12 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>68</v>
       </c>
@@ -6124,7 +6126,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6141,7 +6143,7 @@
         <v>5.28E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -6158,7 +6160,7 @@
         <v>4.0800000000000003E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -6175,7 +6177,7 @@
         <v>3.6799999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -6192,7 +6194,7 @@
         <v>8.3999999999999995E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2</v>
       </c>
@@ -6209,7 +6211,7 @@
         <v>4.1799999999999997E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2</v>
       </c>
@@ -6226,7 +6228,7 @@
         <v>3.7400000000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>4</v>
       </c>
@@ -6243,7 +6245,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>5</v>
       </c>
@@ -6260,7 +6262,7 @@
         <v>2.0400000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>6</v>
       </c>
@@ -6277,7 +6279,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>6</v>
       </c>
@@ -6294,7 +6296,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>6</v>
       </c>
@@ -6311,7 +6313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>6</v>
       </c>
@@ -6328,7 +6330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>9</v>
       </c>
@@ -6345,7 +6347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>9</v>
       </c>
@@ -6362,7 +6364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>4</v>
       </c>
@@ -6379,7 +6381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>12</v>
       </c>
@@ -6396,7 +6398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>12</v>
       </c>
@@ -6413,7 +6415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>12</v>
       </c>
@@ -6430,7 +6432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>12</v>
       </c>
@@ -6447,7 +6449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>14</v>
       </c>
@@ -6464,7 +6466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>16</v>
       </c>
@@ -6481,7 +6483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>15</v>
       </c>
@@ -6498,7 +6500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>18</v>
       </c>
@@ -6515,7 +6517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>19</v>
       </c>
@@ -6532,7 +6534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>10</v>
       </c>
@@ -6549,7 +6551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>10</v>
       </c>
@@ -6566,7 +6568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>10</v>
       </c>
@@ -6583,7 +6585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>10</v>
       </c>
@@ -6600,7 +6602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>21</v>
       </c>
@@ -6617,7 +6619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>15</v>
       </c>
@@ -6634,7 +6636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>22</v>
       </c>
@@ -6651,7 +6653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>23</v>
       </c>
@@ -6668,7 +6670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>24</v>
       </c>
@@ -6685,7 +6687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>25</v>
       </c>
@@ -6702,7 +6704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>25</v>
       </c>
@@ -6719,7 +6721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>28</v>
       </c>
@@ -6736,7 +6738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>27</v>
       </c>
@@ -6753,7 +6755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>27</v>
       </c>
@@ -6770,7 +6772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>29</v>
       </c>
@@ -6787,7 +6789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>8</v>
       </c>
@@ -6804,7 +6806,7 @@
         <v>4.2799999999999998E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Add Jupyter Notebook for generating and saving system analysis graphs
- Implemented data loading from an Excel file containing generator, short-circuit, and frequency data.
- Created four distinct graphs:
  1. Stacked bar chart for generation dispatch.
  2. Line graph for minimum short-circuit current (SCC) with a defined limit.
  3. Line graph for equivalent inertia of the system.
  4. Line graph for Rate of Change of Frequency (RoCoF) with a defined limit.
- Each graph is saved as a PNG file in a specified output directory.
- Added error handling for file loading and graph generation processes.
</commit_message>
<xml_diff>
--- a/Código PAPER/modelo/data/input/datos_finales30.xlsx
+++ b/Código PAPER/modelo/data/input/datos_finales30.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ff7811548ae3acaf/Documentos/GitHub/IEE2985/Código PAPER/modelo/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{980BB2A6-2B7B-574E-91E4-3A6BED000D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA45E218-A98C-4EAD-9062-363AE6CA536C}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{980BB2A6-2B7B-574E-91E4-3A6BED000D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D038A47-A086-4A06-8A07-D5C98C95B34D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{80E02269-A3DD-48C4-A8B7-66D9192E8AAD}"/>
+    <workbookView xWindow="1150" yWindow="620" windowWidth="17730" windowHeight="9020" xr2:uid="{80E02269-A3DD-48C4-A8B7-66D9192E8AAD}"/>
   </bookViews>
   <sheets>
     <sheet name="BUS DATA" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
   <si>
     <t>id</t>
   </si>
@@ -254,6 +254,9 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>Bshunt</t>
   </si>
 </sst>
 </file>
@@ -263,7 +266,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -280,6 +283,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -305,12 +314,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -649,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C404ACF8-4AE1-492F-B81B-865E1642AE83}">
-  <dimension ref="A1:AL67"/>
+  <dimension ref="A1:AM67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H16" workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+    <sheetView tabSelected="1" topLeftCell="J25" workbookViewId="0">
+      <selection activeCell="R32" sqref="R32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -661,7 +671,7 @@
     <col min="10" max="10" width="13.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -704,80 +714,83 @@
       <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" t="s">
+        <v>72</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -787,8 +800,12 @@
       <c r="C2" s="3">
         <v>3</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="D2" s="3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3">
+        <v>20</v>
+      </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -800,8 +817,8 @@
       <c r="N2" s="3">
         <v>2</v>
       </c>
-      <c r="O2">
-        <v>0</v>
+      <c r="O2" s="3">
+        <v>0.01</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -872,8 +889,11 @@
       <c r="AL2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AM2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -916,80 +936,83 @@
       <c r="N3" s="3">
         <v>0.2</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="P3">
         <v>91.131780000000006</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>86.859977999999998</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>82.588176000000004</v>
-      </c>
-      <c r="R3">
-        <v>79.740307999999999</v>
       </c>
       <c r="S3">
         <v>79.740307999999999</v>
       </c>
       <c r="T3">
+        <v>79.740307999999999</v>
+      </c>
+      <c r="U3">
         <v>85.436043999999995</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>99.675385000000006</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>113.914725</v>
       </c>
-      <c r="W3">
+      <c r="X3">
         <v>125.30619799999999</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <v>131.00193400000001</v>
       </c>
-      <c r="Y3">
+      <c r="Z3">
         <v>135.27373600000001</v>
       </c>
-      <c r="Z3">
+      <c r="AA3">
         <v>138.12160499999999</v>
-      </c>
-      <c r="AA3">
-        <v>139.54553899999999</v>
       </c>
       <c r="AB3">
         <v>139.54553899999999</v>
       </c>
       <c r="AC3">
+        <v>139.54553899999999</v>
+      </c>
+      <c r="AD3">
         <v>140.96947299999999</v>
       </c>
-      <c r="AD3">
+      <c r="AE3">
         <v>142.393407</v>
       </c>
-      <c r="AE3">
+      <c r="AF3">
         <v>149.51307700000001</v>
       </c>
-      <c r="AF3">
+      <c r="AG3">
         <v>153.78487899999999</v>
       </c>
-      <c r="AG3">
+      <c r="AH3">
         <v>156.63274699999999</v>
       </c>
-      <c r="AH3">
+      <c r="AI3">
         <v>145.241275</v>
       </c>
-      <c r="AI3">
+      <c r="AJ3">
         <v>135.27373600000001</v>
       </c>
-      <c r="AJ3">
+      <c r="AK3">
         <v>125.30619799999999</v>
       </c>
-      <c r="AK3">
+      <c r="AL3">
         <v>113.914725</v>
       </c>
-      <c r="AL3">
+      <c r="AM3">
         <v>99.675385000000006</v>
       </c>
     </row>
-    <row r="4" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1032,80 +1055,83 @@
       <c r="N4" s="3">
         <v>0.22</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="P4">
         <v>1.8226359999999999</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>1.7372000000000001</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>1.651764</v>
-      </c>
-      <c r="R4">
-        <v>1.5948059999999999</v>
       </c>
       <c r="S4">
         <v>1.5948059999999999</v>
       </c>
       <c r="T4">
+        <v>1.5948059999999999</v>
+      </c>
+      <c r="U4">
         <v>1.7087209999999999</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>1.9935080000000001</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>2.278295</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <v>2.5061239999999998</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>2.6200389999999998</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>2.7054749999999999</v>
       </c>
-      <c r="Z4">
+      <c r="AA4">
         <v>2.762432</v>
-      </c>
-      <c r="AA4">
-        <v>2.7909109999999999</v>
       </c>
       <c r="AB4">
         <v>2.7909109999999999</v>
       </c>
       <c r="AC4">
+        <v>2.7909109999999999</v>
+      </c>
+      <c r="AD4">
         <v>2.8193890000000001</v>
       </c>
-      <c r="AD4">
+      <c r="AE4">
         <v>2.8478680000000001</v>
       </c>
-      <c r="AE4">
+      <c r="AF4">
         <v>2.990262</v>
       </c>
-      <c r="AF4">
+      <c r="AG4">
         <v>3.075698</v>
       </c>
-      <c r="AG4">
+      <c r="AH4">
         <v>3.1326550000000002</v>
       </c>
-      <c r="AH4">
+      <c r="AI4">
         <v>2.9048250000000002</v>
       </c>
-      <c r="AI4">
+      <c r="AJ4">
         <v>2.7054749999999999</v>
       </c>
-      <c r="AJ4">
+      <c r="AK4">
         <v>2.5061239999999998</v>
       </c>
-      <c r="AK4">
+      <c r="AL4">
         <v>2.278295</v>
       </c>
-      <c r="AL4">
+      <c r="AM4">
         <v>1.9935080000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1148,8 +1174,8 @@
       <c r="N5" s="3">
         <v>0.25</v>
       </c>
-      <c r="O5">
-        <v>0</v>
+      <c r="O5" s="3">
+        <v>0.01</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -1220,8 +1246,11 @@
       <c r="AL5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AM5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1264,8 +1293,8 @@
       <c r="N6" s="3">
         <v>0.27</v>
       </c>
-      <c r="O6">
-        <v>0</v>
+      <c r="O6" s="3">
+        <v>0.01</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -1336,8 +1365,11 @@
       <c r="AL6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AM6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1358,8 +1390,8 @@
       <c r="L7" s="3"/>
       <c r="M7" s="4"/>
       <c r="N7" s="3"/>
-      <c r="O7">
-        <v>0</v>
+      <c r="O7" s="3">
+        <v>0.01</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -1430,8 +1462,11 @@
       <c r="AL7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AM7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1452,80 +1487,83 @@
       <c r="L8" s="3"/>
       <c r="M8" s="4"/>
       <c r="N8" s="3"/>
-      <c r="O8">
+      <c r="O8" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="P8">
         <v>21.226111</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <v>20.231137</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>19.236163000000001</v>
-      </c>
-      <c r="R8">
-        <v>18.572846999999999</v>
       </c>
       <c r="S8">
         <v>18.572846999999999</v>
       </c>
       <c r="T8">
+        <v>18.572846999999999</v>
+      </c>
+      <c r="U8">
         <v>19.899478999999999</v>
       </c>
-      <c r="U8">
+      <c r="V8">
         <v>23.216058</v>
       </c>
-      <c r="V8">
+      <c r="W8">
         <v>26.532637999999999</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <v>29.185901999999999</v>
       </c>
-      <c r="X8">
+      <c r="Y8">
         <v>30.512533999999999</v>
       </c>
-      <c r="Y8">
+      <c r="Z8">
         <v>31.507508000000001</v>
       </c>
-      <c r="Z8">
+      <c r="AA8">
         <v>32.170824000000003</v>
-      </c>
-      <c r="AA8">
-        <v>32.502482000000001</v>
       </c>
       <c r="AB8">
         <v>32.502482000000001</v>
       </c>
       <c r="AC8">
+        <v>32.502482000000001</v>
+      </c>
+      <c r="AD8">
         <v>32.834139999999998</v>
       </c>
-      <c r="AD8">
+      <c r="AE8">
         <v>33.165798000000002</v>
       </c>
-      <c r="AE8">
+      <c r="AF8">
         <v>34.824088000000003</v>
       </c>
-      <c r="AF8">
+      <c r="AG8">
         <v>35.819060999999998</v>
       </c>
-      <c r="AG8">
+      <c r="AH8">
         <v>36.482377</v>
       </c>
-      <c r="AH8">
+      <c r="AI8">
         <v>33.829113999999997</v>
       </c>
-      <c r="AI8">
+      <c r="AJ8">
         <v>31.507508000000001</v>
       </c>
-      <c r="AJ8">
+      <c r="AK8">
         <v>29.185901999999999</v>
       </c>
-      <c r="AK8">
+      <c r="AL8">
         <v>26.532637999999999</v>
       </c>
-      <c r="AL8">
+      <c r="AM8">
         <v>23.216058</v>
       </c>
     </row>
-    <row r="9" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1546,8 +1584,8 @@
       <c r="L9" s="3"/>
       <c r="M9" s="4"/>
       <c r="N9" s="3"/>
-      <c r="O9">
-        <v>0</v>
+      <c r="O9" s="3">
+        <v>0.01</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -1618,8 +1656,11 @@
       <c r="AL9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AM9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1640,8 +1681,8 @@
       <c r="L10" s="3"/>
       <c r="M10" s="4"/>
       <c r="N10" s="3"/>
-      <c r="O10">
-        <v>0</v>
+      <c r="O10" s="3">
+        <v>0.01</v>
       </c>
       <c r="P10">
         <v>0</v>
@@ -1712,8 +1753,11 @@
       <c r="AL10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AM10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1734,80 +1778,83 @@
       <c r="L11" s="3"/>
       <c r="M11" s="4"/>
       <c r="N11" s="3"/>
-      <c r="O11">
+      <c r="O11" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="P11">
         <v>5.7716789999999998</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <v>5.5011320000000001</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>5.2305840000000003</v>
-      </c>
-      <c r="R11">
-        <v>5.0502190000000002</v>
       </c>
       <c r="S11">
         <v>5.0502190000000002</v>
       </c>
       <c r="T11">
+        <v>5.0502190000000002</v>
+      </c>
+      <c r="U11">
         <v>5.4109489999999996</v>
       </c>
-      <c r="U11">
+      <c r="V11">
         <v>6.3127740000000001</v>
       </c>
-      <c r="V11">
+      <c r="W11">
         <v>7.2145989999999998</v>
       </c>
-      <c r="W11">
+      <c r="X11">
         <v>7.9360590000000002</v>
       </c>
-      <c r="X11">
+      <c r="Y11">
         <v>8.2967890000000004</v>
       </c>
-      <c r="Y11">
+      <c r="Z11">
         <v>8.5673370000000002</v>
       </c>
-      <c r="Z11">
+      <c r="AA11">
         <v>8.7477020000000003</v>
-      </c>
-      <c r="AA11">
-        <v>8.8378840000000007</v>
       </c>
       <c r="AB11">
         <v>8.8378840000000007</v>
       </c>
       <c r="AC11">
+        <v>8.8378840000000007</v>
+      </c>
+      <c r="AD11">
         <v>8.9280670000000004</v>
       </c>
-      <c r="AD11">
+      <c r="AE11">
         <v>9.0182490000000008</v>
       </c>
-      <c r="AE11">
+      <c r="AF11">
         <v>9.4691620000000007</v>
       </c>
-      <c r="AF11">
+      <c r="AG11">
         <v>9.7397089999999995</v>
       </c>
-      <c r="AG11">
+      <c r="AH11">
         <v>9.9200739999999996</v>
       </c>
-      <c r="AH11">
+      <c r="AI11">
         <v>9.1986139999999992</v>
       </c>
-      <c r="AI11">
+      <c r="AJ11">
         <v>8.5673370000000002</v>
       </c>
-      <c r="AJ11">
+      <c r="AK11">
         <v>7.9360590000000002</v>
       </c>
-      <c r="AK11">
+      <c r="AL11">
         <v>7.2145989999999998</v>
       </c>
-      <c r="AL11">
+      <c r="AM11">
         <v>6.3127740000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1828,8 +1875,8 @@
       <c r="L12" s="3"/>
       <c r="M12" s="4"/>
       <c r="N12" s="3"/>
-      <c r="O12">
-        <v>0</v>
+      <c r="O12" s="3">
+        <v>0.01</v>
       </c>
       <c r="P12">
         <v>0</v>
@@ -1900,8 +1947,11 @@
       <c r="AL12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AM12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1922,80 +1972,83 @@
       <c r="L13" s="3"/>
       <c r="M13" s="4"/>
       <c r="N13" s="3"/>
-      <c r="O13">
+      <c r="O13" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="P13">
         <v>10.859870000000001</v>
       </c>
-      <c r="P13">
+      <c r="Q13">
         <v>10.350814</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>9.8417580000000005</v>
-      </c>
-      <c r="R13">
-        <v>9.5023870000000006</v>
       </c>
       <c r="S13">
         <v>9.5023870000000006</v>
       </c>
       <c r="T13">
+        <v>9.5023870000000006</v>
+      </c>
+      <c r="U13">
         <v>10.181129</v>
       </c>
-      <c r="U13">
+      <c r="V13">
         <v>11.877983</v>
       </c>
-      <c r="V13">
+      <c r="W13">
         <v>13.574838</v>
       </c>
-      <c r="W13">
+      <c r="X13">
         <v>14.932321999999999</v>
       </c>
-      <c r="X13">
+      <c r="Y13">
         <v>15.611064000000001</v>
       </c>
-      <c r="Y13">
+      <c r="Z13">
         <v>16.12012</v>
       </c>
-      <c r="Z13">
+      <c r="AA13">
         <v>16.459491</v>
-      </c>
-      <c r="AA13">
-        <v>16.629176999999999</v>
       </c>
       <c r="AB13">
         <v>16.629176999999999</v>
       </c>
       <c r="AC13">
+        <v>16.629176999999999</v>
+      </c>
+      <c r="AD13">
         <v>16.798862</v>
       </c>
-      <c r="AD13">
+      <c r="AE13">
         <v>16.968547999999998</v>
       </c>
-      <c r="AE13">
+      <c r="AF13">
         <v>17.816974999999999</v>
       </c>
-      <c r="AF13">
+      <c r="AG13">
         <v>18.326031</v>
       </c>
-      <c r="AG13">
+      <c r="AH13">
         <v>18.665402</v>
       </c>
-      <c r="AH13">
+      <c r="AI13">
         <v>17.307918999999998</v>
       </c>
-      <c r="AI13">
+      <c r="AJ13">
         <v>16.12012</v>
       </c>
-      <c r="AJ13">
+      <c r="AK13">
         <v>14.932321999999999</v>
       </c>
-      <c r="AK13">
+      <c r="AL13">
         <v>13.574838</v>
       </c>
-      <c r="AL13">
+      <c r="AM13">
         <v>11.877983</v>
       </c>
     </row>
-    <row r="14" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2016,8 +2069,8 @@
       <c r="L14" s="3"/>
       <c r="M14" s="4"/>
       <c r="N14" s="3"/>
-      <c r="O14">
-        <v>0</v>
+      <c r="O14" s="3">
+        <v>0.01</v>
       </c>
       <c r="P14">
         <v>0</v>
@@ -2088,8 +2141,11 @@
       <c r="AL14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AM14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2110,80 +2166,83 @@
       <c r="L15" s="3"/>
       <c r="M15" s="4"/>
       <c r="N15" s="3"/>
-      <c r="O15">
+      <c r="O15" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="P15">
         <v>5.8855940000000002</v>
       </c>
-      <c r="P15">
+      <c r="Q15">
         <v>5.6097070000000002</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>5.3338200000000002</v>
-      </c>
-      <c r="R15">
-        <v>5.1498949999999999</v>
       </c>
       <c r="S15">
         <v>5.1498949999999999</v>
       </c>
       <c r="T15">
+        <v>5.1498949999999999</v>
+      </c>
+      <c r="U15">
         <v>5.5177449999999997</v>
       </c>
-      <c r="U15">
+      <c r="V15">
         <v>6.4373690000000003</v>
       </c>
-      <c r="V15">
+      <c r="W15">
         <v>7.3569930000000001</v>
       </c>
-      <c r="W15">
+      <c r="X15">
         <v>8.0926919999999996</v>
       </c>
-      <c r="X15">
+      <c r="Y15">
         <v>8.4605420000000002</v>
       </c>
-      <c r="Y15">
+      <c r="Z15">
         <v>8.7364289999999993</v>
       </c>
-      <c r="Z15">
+      <c r="AA15">
         <v>8.9203539999999997</v>
-      </c>
-      <c r="AA15">
-        <v>9.0123160000000002</v>
       </c>
       <c r="AB15">
         <v>9.0123160000000002</v>
       </c>
       <c r="AC15">
+        <v>9.0123160000000002</v>
+      </c>
+      <c r="AD15">
         <v>9.1042780000000008</v>
       </c>
-      <c r="AD15">
+      <c r="AE15">
         <v>9.1962410000000006</v>
       </c>
-      <c r="AE15">
+      <c r="AF15">
         <v>9.656053</v>
       </c>
-      <c r="AF15">
+      <c r="AG15">
         <v>9.9319400000000009</v>
       </c>
-      <c r="AG15">
+      <c r="AH15">
         <v>10.115864999999999</v>
       </c>
-      <c r="AH15">
+      <c r="AI15">
         <v>9.3801659999999991</v>
       </c>
-      <c r="AI15">
+      <c r="AJ15">
         <v>8.7364289999999993</v>
       </c>
-      <c r="AJ15">
+      <c r="AK15">
         <v>8.0926919999999996</v>
       </c>
-      <c r="AK15">
+      <c r="AL15">
         <v>7.3569930000000001</v>
       </c>
-      <c r="AL15">
+      <c r="AM15">
         <v>6.4373690000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2204,80 +2263,83 @@
       <c r="L16" s="3"/>
       <c r="M16" s="4"/>
       <c r="N16" s="3"/>
-      <c r="O16">
+      <c r="O16" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="P16">
         <v>7.8980880000000004</v>
       </c>
-      <c r="P16">
+      <c r="Q16">
         <v>7.5278650000000003</v>
       </c>
-      <c r="Q16">
+      <c r="R16">
         <v>7.1576420000000001</v>
-      </c>
-      <c r="R16">
-        <v>6.9108270000000003</v>
       </c>
       <c r="S16">
         <v>6.9108270000000003</v>
       </c>
       <c r="T16">
+        <v>6.9108270000000003</v>
+      </c>
+      <c r="U16">
         <v>7.4044569999999998</v>
       </c>
-      <c r="U16">
+      <c r="V16">
         <v>8.6385330000000007</v>
       </c>
-      <c r="V16">
+      <c r="W16">
         <v>9.8726099999999999</v>
       </c>
-      <c r="W16">
+      <c r="X16">
         <v>10.859870000000001</v>
       </c>
-      <c r="X16">
+      <c r="Y16">
         <v>11.353501</v>
       </c>
-      <c r="Y16">
+      <c r="Z16">
         <v>11.723724000000001</v>
       </c>
-      <c r="Z16">
+      <c r="AA16">
         <v>11.970539</v>
-      </c>
-      <c r="AA16">
-        <v>12.093947</v>
       </c>
       <c r="AB16">
         <v>12.093947</v>
       </c>
       <c r="AC16">
+        <v>12.093947</v>
+      </c>
+      <c r="AD16">
         <v>12.217354</v>
       </c>
-      <c r="AD16">
+      <c r="AE16">
         <v>12.340762</v>
       </c>
-      <c r="AE16">
+      <c r="AF16">
         <v>12.957800000000001</v>
       </c>
-      <c r="AF16">
+      <c r="AG16">
         <v>13.328023</v>
       </c>
-      <c r="AG16">
+      <c r="AH16">
         <v>13.574838</v>
       </c>
-      <c r="AH16">
+      <c r="AI16">
         <v>12.587577</v>
       </c>
-      <c r="AI16">
+      <c r="AJ16">
         <v>11.723724000000001</v>
       </c>
-      <c r="AJ16">
+      <c r="AK16">
         <v>10.859870000000001</v>
       </c>
-      <c r="AK16">
+      <c r="AL16">
         <v>9.8726099999999999</v>
       </c>
-      <c r="AL16">
+      <c r="AM16">
         <v>8.6385330000000007</v>
       </c>
     </row>
-    <row r="17" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2298,80 +2360,83 @@
       <c r="L17" s="3"/>
       <c r="M17" s="4"/>
       <c r="N17" s="3"/>
-      <c r="O17">
+      <c r="O17" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="P17">
         <v>3.5313560000000002</v>
       </c>
-      <c r="P17">
+      <c r="Q17">
         <v>3.3658239999999999</v>
       </c>
-      <c r="Q17">
+      <c r="R17">
         <v>3.2002920000000001</v>
-      </c>
-      <c r="R17">
-        <v>3.0899369999999999</v>
       </c>
       <c r="S17">
         <v>3.0899369999999999</v>
       </c>
       <c r="T17">
+        <v>3.0899369999999999</v>
+      </c>
+      <c r="U17">
         <v>3.3106469999999999</v>
       </c>
-      <c r="U17">
+      <c r="V17">
         <v>3.8624209999999999</v>
       </c>
-      <c r="V17">
+      <c r="W17">
         <v>4.4141959999999996</v>
       </c>
-      <c r="W17">
+      <c r="X17">
         <v>4.8556150000000002</v>
       </c>
-      <c r="X17">
+      <c r="Y17">
         <v>5.0763249999999998</v>
       </c>
-      <c r="Y17">
+      <c r="Z17">
         <v>5.2418570000000004</v>
       </c>
-      <c r="Z17">
+      <c r="AA17">
         <v>5.3522119999999997</v>
-      </c>
-      <c r="AA17">
-        <v>5.4073900000000004</v>
       </c>
       <c r="AB17">
         <v>5.4073900000000004</v>
       </c>
       <c r="AC17">
+        <v>5.4073900000000004</v>
+      </c>
+      <c r="AD17">
         <v>5.462567</v>
       </c>
-      <c r="AD17">
+      <c r="AE17">
         <v>5.5177449999999997</v>
       </c>
-      <c r="AE17">
+      <c r="AF17">
         <v>5.7936319999999997</v>
       </c>
-      <c r="AF17">
+      <c r="AG17">
         <v>5.9591640000000003</v>
       </c>
-      <c r="AG17">
+      <c r="AH17">
         <v>6.0695189999999997</v>
       </c>
-      <c r="AH17">
+      <c r="AI17">
         <v>5.6280989999999997</v>
       </c>
-      <c r="AI17">
+      <c r="AJ17">
         <v>5.2418570000000004</v>
       </c>
-      <c r="AJ17">
+      <c r="AK17">
         <v>4.8556150000000002</v>
       </c>
-      <c r="AK17">
+      <c r="AL17">
         <v>4.4141959999999996</v>
       </c>
-      <c r="AL17">
+      <c r="AM17">
         <v>3.8624209999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2392,80 +2457,83 @@
       <c r="L18" s="3"/>
       <c r="M18" s="4"/>
       <c r="N18" s="3"/>
-      <c r="O18">
+      <c r="O18" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="P18">
         <v>8.8094049999999999</v>
       </c>
-      <c r="P18">
+      <c r="Q18">
         <v>8.3964649999999992</v>
       </c>
-      <c r="Q18">
+      <c r="R18">
         <v>7.9835240000000001</v>
-      </c>
-      <c r="R18">
-        <v>7.7082300000000004</v>
       </c>
       <c r="S18">
         <v>7.7082300000000004</v>
       </c>
       <c r="T18">
+        <v>7.7082300000000004</v>
+      </c>
+      <c r="U18">
         <v>8.2588179999999998</v>
       </c>
-      <c r="U18">
+      <c r="V18">
         <v>9.6352869999999999</v>
       </c>
-      <c r="V18">
+      <c r="W18">
         <v>11.011756999999999</v>
       </c>
-      <c r="W18">
+      <c r="X18">
         <v>12.112932000000001</v>
       </c>
-      <c r="X18">
+      <c r="Y18">
         <v>12.66352</v>
       </c>
-      <c r="Y18">
+      <c r="Z18">
         <v>13.076461</v>
       </c>
-      <c r="Z18">
+      <c r="AA18">
         <v>13.351755000000001</v>
-      </c>
-      <c r="AA18">
-        <v>13.489402</v>
       </c>
       <c r="AB18">
         <v>13.489402</v>
       </c>
       <c r="AC18">
+        <v>13.489402</v>
+      </c>
+      <c r="AD18">
         <v>13.627049</v>
       </c>
-      <c r="AD18">
+      <c r="AE18">
         <v>13.764696000000001</v>
       </c>
-      <c r="AE18">
+      <c r="AF18">
         <v>14.452931</v>
       </c>
-      <c r="AF18">
+      <c r="AG18">
         <v>14.865872</v>
       </c>
-      <c r="AG18">
+      <c r="AH18">
         <v>15.141166</v>
       </c>
-      <c r="AH18">
+      <c r="AI18">
         <v>14.03999</v>
       </c>
-      <c r="AI18">
+      <c r="AJ18">
         <v>13.076461</v>
       </c>
-      <c r="AJ18">
+      <c r="AK18">
         <v>12.112932000000001</v>
       </c>
-      <c r="AK18">
+      <c r="AL18">
         <v>11.011756999999999</v>
       </c>
-      <c r="AL18">
+      <c r="AM18">
         <v>9.6352869999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2486,80 +2554,83 @@
       <c r="L19" s="3"/>
       <c r="M19" s="4"/>
       <c r="N19" s="3"/>
-      <c r="O19">
+      <c r="O19" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="P19">
         <v>3.2275839999999998</v>
       </c>
-      <c r="P19">
+      <c r="Q19">
         <v>3.0762909999999999</v>
       </c>
-      <c r="Q19">
+      <c r="R19">
         <v>2.924998</v>
-      </c>
-      <c r="R19">
-        <v>2.8241360000000002</v>
       </c>
       <c r="S19">
         <v>2.8241360000000002</v>
       </c>
       <c r="T19">
+        <v>2.8241360000000002</v>
+      </c>
+      <c r="U19">
         <v>3.0258600000000002</v>
       </c>
-      <c r="U19">
+      <c r="V19">
         <v>3.53017</v>
       </c>
-      <c r="V19">
+      <c r="W19">
         <v>4.0344800000000003</v>
       </c>
-      <c r="W19">
+      <c r="X19">
         <v>4.4379280000000003</v>
       </c>
-      <c r="X19">
+      <c r="Y19">
         <v>4.6396519999999999</v>
       </c>
-      <c r="Y19">
+      <c r="Z19">
         <v>4.7909449999999998</v>
       </c>
-      <c r="Z19">
+      <c r="AA19">
         <v>4.891807</v>
-      </c>
-      <c r="AA19">
-        <v>4.9422379999999997</v>
       </c>
       <c r="AB19">
         <v>4.9422379999999997</v>
       </c>
       <c r="AC19">
+        <v>4.9422379999999997</v>
+      </c>
+      <c r="AD19">
         <v>4.9926690000000002</v>
       </c>
-      <c r="AD19">
+      <c r="AE19">
         <v>5.0430999999999999</v>
       </c>
-      <c r="AE19">
+      <c r="AF19">
         <v>5.295255</v>
       </c>
-      <c r="AF19">
+      <c r="AG19">
         <v>5.4465479999999999</v>
       </c>
-      <c r="AG19">
+      <c r="AH19">
         <v>5.5474100000000002</v>
       </c>
-      <c r="AH19">
+      <c r="AI19">
         <v>5.1439620000000001</v>
       </c>
-      <c r="AI19">
+      <c r="AJ19">
         <v>4.7909449999999998</v>
       </c>
-      <c r="AJ19">
+      <c r="AK19">
         <v>4.4379280000000003</v>
       </c>
-      <c r="AK19">
+      <c r="AL19">
         <v>4.0344800000000003</v>
       </c>
-      <c r="AL19">
+      <c r="AM19">
         <v>3.53017</v>
       </c>
     </row>
-    <row r="20" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2580,80 +2651,83 @@
       <c r="L20" s="3"/>
       <c r="M20" s="4"/>
       <c r="N20" s="3"/>
-      <c r="O20">
+      <c r="O20" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="P20">
         <v>8.8094049999999999</v>
       </c>
-      <c r="P20">
+      <c r="Q20">
         <v>8.3964649999999992</v>
       </c>
-      <c r="Q20">
+      <c r="R20">
         <v>7.9835240000000001</v>
-      </c>
-      <c r="R20">
-        <v>7.7082300000000004</v>
       </c>
       <c r="S20">
         <v>7.7082300000000004</v>
       </c>
       <c r="T20">
+        <v>7.7082300000000004</v>
+      </c>
+      <c r="U20">
         <v>8.2588179999999998</v>
       </c>
-      <c r="U20">
+      <c r="V20">
         <v>9.6352869999999999</v>
       </c>
-      <c r="V20">
+      <c r="W20">
         <v>11.011756999999999</v>
       </c>
-      <c r="W20">
+      <c r="X20">
         <v>12.112932000000001</v>
       </c>
-      <c r="X20">
+      <c r="Y20">
         <v>12.66352</v>
       </c>
-      <c r="Y20">
+      <c r="Z20">
         <v>13.076461</v>
       </c>
-      <c r="Z20">
+      <c r="AA20">
         <v>13.351755000000001</v>
-      </c>
-      <c r="AA20">
-        <v>13.489402</v>
       </c>
       <c r="AB20">
         <v>13.489402</v>
       </c>
       <c r="AC20">
+        <v>13.489402</v>
+      </c>
+      <c r="AD20">
         <v>13.627049</v>
       </c>
-      <c r="AD20">
+      <c r="AE20">
         <v>13.764696000000001</v>
       </c>
-      <c r="AE20">
+      <c r="AF20">
         <v>14.452931</v>
       </c>
-      <c r="AF20">
+      <c r="AG20">
         <v>14.865872</v>
       </c>
-      <c r="AG20">
+      <c r="AH20">
         <v>15.141166</v>
       </c>
-      <c r="AH20">
+      <c r="AI20">
         <v>14.03999</v>
       </c>
-      <c r="AI20">
+      <c r="AJ20">
         <v>13.076461</v>
       </c>
-      <c r="AJ20">
+      <c r="AK20">
         <v>12.112932000000001</v>
       </c>
-      <c r="AK20">
+      <c r="AL20">
         <v>11.011756999999999</v>
       </c>
-      <c r="AL20">
+      <c r="AM20">
         <v>9.6352869999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2674,80 +2748,83 @@
       <c r="L21" s="3"/>
       <c r="M21" s="4"/>
       <c r="N21" s="3"/>
-      <c r="O21">
+      <c r="O21" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="P21">
         <v>2.0884369999999999</v>
       </c>
-      <c r="P21">
+      <c r="Q21">
         <v>1.9905409999999999</v>
       </c>
-      <c r="Q21">
+      <c r="R21">
         <v>1.8926460000000001</v>
-      </c>
-      <c r="R21">
-        <v>1.8273820000000001</v>
       </c>
       <c r="S21">
         <v>1.8273820000000001</v>
       </c>
       <c r="T21">
+        <v>1.8273820000000001</v>
+      </c>
+      <c r="U21">
         <v>1.9579089999999999</v>
       </c>
-      <c r="U21">
+      <c r="V21">
         <v>2.2842280000000001</v>
       </c>
-      <c r="V21">
+      <c r="W21">
         <v>2.6105459999999998</v>
       </c>
-      <c r="W21">
+      <c r="X21">
         <v>2.8715999999999999</v>
       </c>
-      <c r="X21">
+      <c r="Y21">
         <v>3.0021279999999999</v>
       </c>
-      <c r="Y21">
+      <c r="Z21">
         <v>3.1000230000000002</v>
       </c>
-      <c r="Z21">
+      <c r="AA21">
         <v>3.1652870000000002</v>
-      </c>
-      <c r="AA21">
-        <v>3.1979190000000002</v>
       </c>
       <c r="AB21">
         <v>3.1979190000000002</v>
       </c>
       <c r="AC21">
+        <v>3.1979190000000002</v>
+      </c>
+      <c r="AD21">
         <v>3.23055</v>
       </c>
-      <c r="AD21">
+      <c r="AE21">
         <v>3.263182</v>
       </c>
-      <c r="AE21">
+      <c r="AF21">
         <v>3.4263409999999999</v>
       </c>
-      <c r="AF21">
+      <c r="AG21">
         <v>3.5242369999999998</v>
       </c>
-      <c r="AG21">
+      <c r="AH21">
         <v>3.5895000000000001</v>
       </c>
-      <c r="AH21">
+      <c r="AI21">
         <v>3.328446</v>
       </c>
-      <c r="AI21">
+      <c r="AJ21">
         <v>3.1000230000000002</v>
       </c>
-      <c r="AJ21">
+      <c r="AK21">
         <v>2.8715999999999999</v>
       </c>
-      <c r="AK21">
+      <c r="AL21">
         <v>2.6105459999999998</v>
       </c>
-      <c r="AL21">
+      <c r="AM21">
         <v>2.2842280000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2768,80 +2845,83 @@
       <c r="L22" s="3"/>
       <c r="M22" s="4"/>
       <c r="N22" s="3"/>
-      <c r="O22">
+      <c r="O22" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="P22">
         <v>17.163152</v>
       </c>
-      <c r="P22">
+      <c r="Q22">
         <v>16.358629000000001</v>
       </c>
-      <c r="Q22">
+      <c r="R22">
         <v>15.554106000000001</v>
-      </c>
-      <c r="R22">
-        <v>15.017758000000001</v>
       </c>
       <c r="S22">
         <v>15.017758000000001</v>
       </c>
       <c r="T22">
+        <v>15.017758000000001</v>
+      </c>
+      <c r="U22">
         <v>16.090454999999999</v>
       </c>
-      <c r="U22">
+      <c r="V22">
         <v>18.772196999999998</v>
       </c>
-      <c r="V22">
+      <c r="W22">
         <v>21.453939999999999</v>
       </c>
-      <c r="W22">
+      <c r="X22">
         <v>23.599333999999999</v>
       </c>
-      <c r="X22">
+      <c r="Y22">
         <v>24.672031</v>
       </c>
-      <c r="Y22">
+      <c r="Z22">
         <v>25.476554</v>
       </c>
-      <c r="Z22">
+      <c r="AA22">
         <v>26.012902</v>
-      </c>
-      <c r="AA22">
-        <v>26.281075999999999</v>
       </c>
       <c r="AB22">
         <v>26.281075999999999</v>
       </c>
       <c r="AC22">
+        <v>26.281075999999999</v>
+      </c>
+      <c r="AD22">
         <v>26.549251000000002</v>
       </c>
-      <c r="AD22">
+      <c r="AE22">
         <v>26.817425</v>
       </c>
-      <c r="AE22">
+      <c r="AF22">
         <v>28.158296</v>
       </c>
-      <c r="AF22">
+      <c r="AG22">
         <v>28.962819</v>
       </c>
-      <c r="AG22">
+      <c r="AH22">
         <v>29.499167</v>
       </c>
-      <c r="AH22">
+      <c r="AI22">
         <v>27.353773</v>
       </c>
-      <c r="AI22">
+      <c r="AJ22">
         <v>25.476554</v>
       </c>
-      <c r="AJ22">
+      <c r="AK22">
         <v>23.599333999999999</v>
       </c>
-      <c r="AK22">
+      <c r="AL22">
         <v>21.453939999999999</v>
       </c>
-      <c r="AL22">
+      <c r="AM22">
         <v>18.772196999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -2862,8 +2942,8 @@
       <c r="L23" s="3"/>
       <c r="M23" s="4"/>
       <c r="N23" s="3"/>
-      <c r="O23">
-        <v>0</v>
+      <c r="O23" s="3">
+        <v>0.01</v>
       </c>
       <c r="P23">
         <v>0</v>
@@ -2934,8 +3014,11 @@
       <c r="AL23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AM23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -2945,8 +3028,12 @@
       <c r="C24" s="3">
         <v>3</v>
       </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3">
+        <v>20</v>
+      </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -2958,80 +3045,83 @@
       <c r="N24" s="3">
         <v>2</v>
       </c>
-      <c r="O24">
+      <c r="O24" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="P24">
         <v>3.2275839999999998</v>
       </c>
-      <c r="P24">
+      <c r="Q24">
         <v>3.0762909999999999</v>
       </c>
-      <c r="Q24">
+      <c r="R24">
         <v>2.924998</v>
-      </c>
-      <c r="R24">
-        <v>2.8241360000000002</v>
       </c>
       <c r="S24">
         <v>2.8241360000000002</v>
       </c>
       <c r="T24">
+        <v>2.8241360000000002</v>
+      </c>
+      <c r="U24">
         <v>3.0258600000000002</v>
       </c>
-      <c r="U24">
+      <c r="V24">
         <v>3.53017</v>
       </c>
-      <c r="V24">
+      <c r="W24">
         <v>4.0344800000000003</v>
       </c>
-      <c r="W24">
+      <c r="X24">
         <v>4.4379280000000003</v>
       </c>
-      <c r="X24">
+      <c r="Y24">
         <v>4.6396519999999999</v>
       </c>
-      <c r="Y24">
+      <c r="Z24">
         <v>4.7909449999999998</v>
       </c>
-      <c r="Z24">
+      <c r="AA24">
         <v>4.891807</v>
-      </c>
-      <c r="AA24">
-        <v>4.9422379999999997</v>
       </c>
       <c r="AB24">
         <v>4.9422379999999997</v>
       </c>
       <c r="AC24">
+        <v>4.9422379999999997</v>
+      </c>
+      <c r="AD24">
         <v>4.9926690000000002</v>
       </c>
-      <c r="AD24">
+      <c r="AE24">
         <v>5.0430999999999999</v>
       </c>
-      <c r="AE24">
+      <c r="AF24">
         <v>5.295255</v>
       </c>
-      <c r="AF24">
+      <c r="AG24">
         <v>5.4465479999999999</v>
       </c>
-      <c r="AG24">
+      <c r="AH24">
         <v>5.5474100000000002</v>
       </c>
-      <c r="AH24">
+      <c r="AI24">
         <v>5.1439620000000001</v>
       </c>
-      <c r="AI24">
+      <c r="AJ24">
         <v>4.7909449999999998</v>
       </c>
-      <c r="AJ24">
+      <c r="AK24">
         <v>4.4379280000000003</v>
       </c>
-      <c r="AK24">
+      <c r="AL24">
         <v>4.0344800000000003</v>
       </c>
-      <c r="AL24">
+      <c r="AM24">
         <v>3.53017</v>
       </c>
     </row>
-    <row r="25" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -3052,80 +3142,83 @@
       <c r="L25" s="3"/>
       <c r="M25" s="4"/>
       <c r="N25" s="3"/>
-      <c r="O25">
+      <c r="O25" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="P25">
         <v>7.9740310000000001</v>
       </c>
-      <c r="P25">
+      <c r="Q25">
         <v>7.6002479999999997</v>
       </c>
-      <c r="Q25">
+      <c r="R25">
         <v>7.2264650000000001</v>
-      </c>
-      <c r="R25">
-        <v>6.977277</v>
       </c>
       <c r="S25">
         <v>6.977277</v>
       </c>
       <c r="T25">
+        <v>6.977277</v>
+      </c>
+      <c r="U25">
         <v>7.4756539999999996</v>
       </c>
-      <c r="U25">
+      <c r="V25">
         <v>8.7215959999999999</v>
       </c>
-      <c r="V25">
+      <c r="W25">
         <v>9.9675379999999993</v>
       </c>
-      <c r="W25">
+      <c r="X25">
         <v>10.964292</v>
       </c>
-      <c r="X25">
+      <c r="Y25">
         <v>11.462669</v>
       </c>
-      <c r="Y25">
+      <c r="Z25">
         <v>11.836452</v>
       </c>
-      <c r="Z25">
+      <c r="AA25">
         <v>12.08564</v>
-      </c>
-      <c r="AA25">
-        <v>12.210235000000001</v>
       </c>
       <c r="AB25">
         <v>12.210235000000001</v>
       </c>
       <c r="AC25">
+        <v>12.210235000000001</v>
+      </c>
+      <c r="AD25">
         <v>12.334828999999999</v>
       </c>
-      <c r="AD25">
+      <c r="AE25">
         <v>12.459422999999999</v>
       </c>
-      <c r="AE25">
+      <c r="AF25">
         <v>13.082394000000001</v>
       </c>
-      <c r="AF25">
+      <c r="AG25">
         <v>13.456177</v>
       </c>
-      <c r="AG25">
+      <c r="AH25">
         <v>13.705365</v>
       </c>
-      <c r="AH25">
+      <c r="AI25">
         <v>12.708612</v>
       </c>
-      <c r="AI25">
+      <c r="AJ25">
         <v>11.836452</v>
       </c>
-      <c r="AJ25">
+      <c r="AK25">
         <v>10.964292</v>
       </c>
-      <c r="AK25">
+      <c r="AL25">
         <v>9.9675379999999993</v>
       </c>
-      <c r="AL25">
+      <c r="AM25">
         <v>8.7215959999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -3146,8 +3239,8 @@
       <c r="L26" s="3"/>
       <c r="M26" s="4"/>
       <c r="N26" s="3"/>
-      <c r="O26">
-        <v>0</v>
+      <c r="O26" s="3">
+        <v>0.01</v>
       </c>
       <c r="P26">
         <v>0</v>
@@ -3218,8 +3311,11 @@
       <c r="AL26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:38" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="AM26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:39" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -3229,8 +3325,12 @@
       <c r="C27" s="3">
         <v>3</v>
       </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
+      <c r="D27" s="3">
+        <v>0</v>
+      </c>
+      <c r="E27" s="3">
+        <v>20</v>
+      </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -3242,80 +3342,83 @@
       <c r="N27" s="3">
         <v>2</v>
       </c>
-      <c r="O27">
+      <c r="O27" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="P27">
         <v>3.5313560000000002</v>
       </c>
-      <c r="P27">
+      <c r="Q27">
         <v>3.3658239999999999</v>
       </c>
-      <c r="Q27">
+      <c r="R27">
         <v>3.2002920000000001</v>
-      </c>
-      <c r="R27">
-        <v>3.0899369999999999</v>
       </c>
       <c r="S27">
         <v>3.0899369999999999</v>
       </c>
       <c r="T27">
+        <v>3.0899369999999999</v>
+      </c>
+      <c r="U27">
         <v>3.3106469999999999</v>
       </c>
-      <c r="U27">
+      <c r="V27">
         <v>3.8624209999999999</v>
       </c>
-      <c r="V27">
+      <c r="W27">
         <v>4.4141959999999996</v>
       </c>
-      <c r="W27">
+      <c r="X27">
         <v>4.8556150000000002</v>
       </c>
-      <c r="X27">
+      <c r="Y27">
         <v>5.0763249999999998</v>
       </c>
-      <c r="Y27">
+      <c r="Z27">
         <v>5.2418570000000004</v>
       </c>
-      <c r="Z27">
+      <c r="AA27">
         <v>5.3522119999999997</v>
-      </c>
-      <c r="AA27">
-        <v>5.4073900000000004</v>
       </c>
       <c r="AB27">
         <v>5.4073900000000004</v>
       </c>
       <c r="AC27">
+        <v>5.4073900000000004</v>
+      </c>
+      <c r="AD27">
         <v>5.462567</v>
       </c>
-      <c r="AD27">
+      <c r="AE27">
         <v>5.5177449999999997</v>
       </c>
-      <c r="AE27">
+      <c r="AF27">
         <v>5.7936319999999997</v>
       </c>
-      <c r="AF27">
+      <c r="AG27">
         <v>5.9591640000000003</v>
       </c>
-      <c r="AG27">
+      <c r="AH27">
         <v>6.0695189999999997</v>
       </c>
-      <c r="AH27">
+      <c r="AI27">
         <v>5.6280989999999997</v>
       </c>
-      <c r="AI27">
+      <c r="AJ27">
         <v>5.2418570000000004</v>
       </c>
-      <c r="AJ27">
+      <c r="AK27">
         <v>4.8556150000000002</v>
       </c>
-      <c r="AK27">
+      <c r="AL27">
         <v>4.4141959999999996</v>
       </c>
-      <c r="AL27">
+      <c r="AM27">
         <v>3.8624209999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:38" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:39" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -3358,8 +3461,8 @@
       <c r="N28" s="3">
         <v>0.26</v>
       </c>
-      <c r="O28">
-        <v>0</v>
+      <c r="O28" s="3">
+        <v>0.01</v>
       </c>
       <c r="P28">
         <v>0</v>
@@ -3430,8 +3533,11 @@
       <c r="AL28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:38" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="AM28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:39" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -3452,8 +3558,8 @@
       <c r="L29" s="3"/>
       <c r="M29" s="4"/>
       <c r="N29" s="3"/>
-      <c r="O29">
-        <v>0</v>
+      <c r="O29" s="3">
+        <v>0.01</v>
       </c>
       <c r="P29">
         <v>0</v>
@@ -3524,8 +3630,11 @@
       <c r="AL29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:38" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="AM29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:39" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -3546,80 +3655,83 @@
       <c r="L30" s="3"/>
       <c r="M30" s="4"/>
       <c r="N30" s="3"/>
-      <c r="O30">
+      <c r="O30" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="P30">
         <v>2.278295</v>
       </c>
-      <c r="P30">
+      <c r="Q30">
         <v>2.1714989999999998</v>
       </c>
-      <c r="Q30">
+      <c r="R30">
         <v>2.0647039999999999</v>
-      </c>
-      <c r="R30">
-        <v>1.9935080000000001</v>
       </c>
       <c r="S30">
         <v>1.9935080000000001</v>
       </c>
       <c r="T30">
+        <v>1.9935080000000001</v>
+      </c>
+      <c r="U30">
         <v>2.135901</v>
       </c>
-      <c r="U30">
+      <c r="V30">
         <v>2.4918849999999999</v>
       </c>
-      <c r="V30">
+      <c r="W30">
         <v>2.8478680000000001</v>
       </c>
-      <c r="W30">
+      <c r="X30">
         <v>3.1326550000000002</v>
       </c>
-      <c r="X30">
+      <c r="Y30">
         <v>3.275048</v>
       </c>
-      <c r="Y30">
+      <c r="Z30">
         <v>3.3818429999999999</v>
       </c>
-      <c r="Z30">
+      <c r="AA30">
         <v>3.4530400000000001</v>
-      </c>
-      <c r="AA30">
-        <v>3.4886379999999999</v>
       </c>
       <c r="AB30">
         <v>3.4886379999999999</v>
       </c>
       <c r="AC30">
+        <v>3.4886379999999999</v>
+      </c>
+      <c r="AD30">
         <v>3.5242369999999998</v>
       </c>
-      <c r="AD30">
+      <c r="AE30">
         <v>3.5598350000000001</v>
       </c>
-      <c r="AE30">
+      <c r="AF30">
         <v>3.7378269999999998</v>
       </c>
-      <c r="AF30">
+      <c r="AG30">
         <v>3.8446220000000002</v>
       </c>
-      <c r="AG30">
+      <c r="AH30">
         <v>3.9158189999999999</v>
       </c>
-      <c r="AH30">
+      <c r="AI30">
         <v>3.6310319999999998</v>
       </c>
-      <c r="AI30">
+      <c r="AJ30">
         <v>3.3818429999999999</v>
       </c>
-      <c r="AJ30">
+      <c r="AK30">
         <v>3.1326550000000002</v>
       </c>
-      <c r="AK30">
+      <c r="AL30">
         <v>2.8478680000000001</v>
       </c>
-      <c r="AL30">
+      <c r="AM30">
         <v>2.4918849999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:38" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:39" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -3638,7 +3750,7 @@
       <c r="F31" s="3">
         <v>28</v>
       </c>
-      <c r="G31" s="3">
+      <c r="G31" s="5">
         <v>15</v>
       </c>
       <c r="H31" s="3">
@@ -3662,8 +3774,8 @@
       <c r="N31" s="3">
         <v>0.28000000000000003</v>
       </c>
-      <c r="O31">
-        <v>0</v>
+      <c r="O31" s="3">
+        <v>0.01</v>
       </c>
       <c r="P31">
         <v>0</v>
@@ -3734,8 +3846,36 @@
       <c r="AL31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:38" ht="14.5" x14ac:dyDescent="0.35"/>
+      <c r="AM31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:39" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+      <c r="Y32" s="1"/>
+      <c r="Z32" s="1"/>
+      <c r="AA32" s="1"/>
+      <c r="AB32" s="1"/>
+      <c r="AC32" s="1"/>
+      <c r="AD32" s="1"/>
+      <c r="AE32" s="1"/>
+      <c r="AF32" s="1"/>
+      <c r="AG32" s="1"/>
+      <c r="AH32" s="1"/>
+      <c r="AI32" s="1"/>
+      <c r="AJ32" s="1"/>
+      <c r="AK32" s="1"/>
+      <c r="AL32" s="1"/>
+      <c r="AM32" s="1"/>
+    </row>
     <row r="37" spans="6:6" ht="14.5" x14ac:dyDescent="0.35"/>
     <row r="38" spans="6:6" ht="14.5" x14ac:dyDescent="0.35">
       <c r="F38" s="2"/>

</xml_diff>

<commit_message>
Perfiles con variación de intregración IBGs
27% de integración muere
</commit_message>
<xml_diff>
--- a/Código PAPER/modelo/data/input/datos_finales30.xlsx
+++ b/Código PAPER/modelo/data/input/datos_finales30.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ff7811548ae3acaf/Documentos/GitHub/IEE2985/Código PAPER/modelo/data/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camilomerino/Documents/IPre/Código PAPER/modelo/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{980BB2A6-2B7B-574E-91E4-3A6BED000D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D038A47-A086-4A06-8A07-D5C98C95B34D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE8E838-AD85-3340-B827-4EEEABE0BD76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1150" yWindow="620" windowWidth="17730" windowHeight="9020" xr2:uid="{80E02269-A3DD-48C4-A8B7-66D9192E8AAD}"/>
+    <workbookView xWindow="160" yWindow="660" windowWidth="38080" windowHeight="20780" xr2:uid="{80E02269-A3DD-48C4-A8B7-66D9192E8AAD}"/>
   </bookViews>
   <sheets>
     <sheet name="BUS DATA" sheetId="1" r:id="rId1"/>
@@ -336,10 +336,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -661,17 +657,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C404ACF8-4AE1-492F-B81B-865E1642AE83}">
   <dimension ref="A1:AM67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J25" workbookViewId="0">
-      <selection activeCell="R32" sqref="R32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.6328125" customWidth="1"/>
-    <col min="10" max="10" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -790,7 +786,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -893,7 +889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -907,7 +903,7 @@
         <v>50</v>
       </c>
       <c r="E3" s="3">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="F3" s="3">
         <v>21</v>
@@ -1012,7 +1008,7 @@
         <v>99.675385000000006</v>
       </c>
     </row>
-    <row r="4" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1131,7 +1127,7 @@
         <v>1.9935080000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1250,7 +1246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1264,7 +1260,7 @@
         <v>10</v>
       </c>
       <c r="E6" s="3">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="F6" s="3">
         <v>27</v>
@@ -1369,7 +1365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1466,7 +1462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1563,7 +1559,7 @@
         <v>23.216058</v>
       </c>
     </row>
-    <row r="9" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1660,7 +1656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1757,7 +1753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1854,7 +1850,7 @@
         <v>6.3127740000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1951,7 +1947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -2048,7 +2044,7 @@
         <v>11.877983</v>
       </c>
     </row>
-    <row r="14" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -2145,7 +2141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -2242,7 +2238,7 @@
         <v>6.4373690000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2339,7 +2335,7 @@
         <v>8.6385330000000007</v>
       </c>
     </row>
-    <row r="17" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -2436,7 +2432,7 @@
         <v>3.8624209999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -2533,7 +2529,7 @@
         <v>9.6352869999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -2630,7 +2626,7 @@
         <v>3.53017</v>
       </c>
     </row>
-    <row r="20" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -2727,7 +2723,7 @@
         <v>9.6352869999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -2824,7 +2820,7 @@
         <v>2.2842280000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -2921,7 +2917,7 @@
         <v>18.772196999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -3018,7 +3014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -3121,7 +3117,7 @@
         <v>3.53017</v>
       </c>
     </row>
-    <row r="25" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -3218,7 +3214,7 @@
         <v>8.7215959999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -3315,7 +3311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:39" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -3418,7 +3414,7 @@
         <v>3.8624209999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:39" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -3537,7 +3533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:39" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -3634,7 +3630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:39" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -3731,7 +3727,7 @@
         <v>2.4918849999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:39" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -3745,7 +3741,7 @@
         <v>10</v>
       </c>
       <c r="E31" s="3">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="F31" s="3">
         <v>28</v>
@@ -3850,7 +3846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:39" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.2">
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
@@ -3876,39 +3872,39 @@
       <c r="AL32" s="1"/>
       <c r="AM32" s="1"/>
     </row>
-    <row r="37" spans="6:6" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="38" spans="6:6" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="6:6" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F38" s="2"/>
     </row>
-    <row r="39" spans="6:6" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="40" spans="6:6" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="41" spans="6:6" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="42" spans="6:6" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="43" spans="6:6" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="44" spans="6:6" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="45" spans="6:6" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="46" spans="6:6" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="47" spans="6:6" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="48" spans="6:6" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="49" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="50" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="51" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="52" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="53" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="54" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="55" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="56" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="57" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="58" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="59" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="60" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="61" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="62" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="63" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="64" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="65" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="66" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="67" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="6:6" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="6:6" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="6:6" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="6:6" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="6:6" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="6:6" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="6:6" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="6:6" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="6:6" x14ac:dyDescent="0.2"/>
+    <row r="49" x14ac:dyDescent="0.2"/>
+    <row r="50" x14ac:dyDescent="0.2"/>
+    <row r="51" x14ac:dyDescent="0.2"/>
+    <row r="52" x14ac:dyDescent="0.2"/>
+    <row r="53" x14ac:dyDescent="0.2"/>
+    <row r="54" x14ac:dyDescent="0.2"/>
+    <row r="55" x14ac:dyDescent="0.2"/>
+    <row r="56" x14ac:dyDescent="0.2"/>
+    <row r="57" x14ac:dyDescent="0.2"/>
+    <row r="58" x14ac:dyDescent="0.2"/>
+    <row r="59" x14ac:dyDescent="0.2"/>
+    <row r="60" x14ac:dyDescent="0.2"/>
+    <row r="61" x14ac:dyDescent="0.2"/>
+    <row r="62" x14ac:dyDescent="0.2"/>
+    <row r="63" x14ac:dyDescent="0.2"/>
+    <row r="64" x14ac:dyDescent="0.2"/>
+    <row r="65" x14ac:dyDescent="0.2"/>
+    <row r="66" x14ac:dyDescent="0.2"/>
+    <row r="67" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3923,9 +3919,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>0</v>
       </c>
@@ -3999,7 +3995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -4073,7 +4069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1.488</v>
       </c>
@@ -4147,7 +4143,7 @@
         <v>1.488</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>4.7119999999999997</v>
       </c>
@@ -4221,7 +4217,7 @@
         <v>4.7119999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0</v>
       </c>
@@ -4295,7 +4291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0</v>
       </c>
@@ -4369,7 +4365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>14.135999999999999</v>
       </c>
@@ -4443,7 +4439,7 @@
         <v>14.135999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0</v>
       </c>
@@ -4517,7 +4513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0</v>
       </c>
@@ -4591,7 +4587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3.5960000000000001</v>
       </c>
@@ -4665,7 +4661,7 @@
         <v>3.5960000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>0</v>
       </c>
@@ -4733,7 +4729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>6.944</v>
       </c>
@@ -4807,7 +4803,7 @@
         <v>6.944</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>0</v>
       </c>
@@ -4875,7 +4871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>3.8439999999999999</v>
       </c>
@@ -4949,7 +4945,7 @@
         <v>3.8439999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>5.0839999999999996</v>
       </c>
@@ -5023,7 +5019,7 @@
         <v>5.0839999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2.17</v>
       </c>
@@ -5097,7 +5093,7 @@
         <v>2.17</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>5.58</v>
       </c>
@@ -5171,7 +5167,7 @@
         <v>5.58</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1.984</v>
       </c>
@@ -5245,7 +5241,7 @@
         <v>1.984</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>5.89</v>
       </c>
@@ -5319,7 +5315,7 @@
         <v>5.89</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1.3640000000000001</v>
       </c>
@@ -5393,7 +5389,7 @@
         <v>1.3640000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>10.85</v>
       </c>
@@ -5467,7 +5463,7 @@
         <v>10.85</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>0</v>
       </c>
@@ -5541,7 +5537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1.984</v>
       </c>
@@ -5615,7 +5611,7 @@
         <v>1.984</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>5.3940000000000001</v>
       </c>
@@ -5689,7 +5685,7 @@
         <v>5.3940000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>0</v>
       </c>
@@ -5763,7 +5759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2.17</v>
       </c>
@@ -5837,7 +5833,7 @@
         <v>2.17</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>0</v>
       </c>
@@ -5911,7 +5907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>0</v>
       </c>
@@ -5985,7 +5981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1.488</v>
       </c>
@@ -6059,7 +6055,7 @@
         <v>1.488</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>6.5720000000000001</v>
       </c>
@@ -6133,7 +6129,7 @@
         <v>6.5720000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31">
         <f>SUM(A1:A30)</f>
         <v>85.25</v>
@@ -6244,12 +6240,12 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>68</v>
       </c>
@@ -6266,7 +6262,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6283,7 +6279,7 @@
         <v>5.28E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -6300,7 +6296,7 @@
         <v>4.0800000000000003E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -6317,7 +6313,7 @@
         <v>3.6799999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -6334,7 +6330,7 @@
         <v>8.3999999999999995E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -6351,7 +6347,7 @@
         <v>4.1799999999999997E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2</v>
       </c>
@@ -6368,7 +6364,7 @@
         <v>3.7400000000000003E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -6385,7 +6381,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
@@ -6402,7 +6398,7 @@
         <v>2.0400000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
@@ -6419,7 +6415,7 @@
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>6</v>
       </c>
@@ -6436,7 +6432,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>6</v>
       </c>
@@ -6453,7 +6449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>6</v>
       </c>
@@ -6470,7 +6466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>9</v>
       </c>
@@ -6487,7 +6483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>9</v>
       </c>
@@ -6504,7 +6500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>4</v>
       </c>
@@ -6521,7 +6517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>12</v>
       </c>
@@ -6538,7 +6534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>12</v>
       </c>
@@ -6555,7 +6551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>12</v>
       </c>
@@ -6572,7 +6568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>12</v>
       </c>
@@ -6589,7 +6585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>14</v>
       </c>
@@ -6606,7 +6602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>16</v>
       </c>
@@ -6623,7 +6619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>15</v>
       </c>
@@ -6640,7 +6636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>18</v>
       </c>
@@ -6657,7 +6653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>19</v>
       </c>
@@ -6674,7 +6670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>10</v>
       </c>
@@ -6691,7 +6687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>10</v>
       </c>
@@ -6708,7 +6704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>10</v>
       </c>
@@ -6725,7 +6721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>10</v>
       </c>
@@ -6742,7 +6738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>21</v>
       </c>
@@ -6759,7 +6755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>15</v>
       </c>
@@ -6776,7 +6772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>22</v>
       </c>
@@ -6793,7 +6789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>23</v>
       </c>
@@ -6810,7 +6806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>24</v>
       </c>
@@ -6827,7 +6823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>25</v>
       </c>
@@ -6844,7 +6840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>25</v>
       </c>
@@ -6861,7 +6857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>28</v>
       </c>
@@ -6878,7 +6874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>27</v>
       </c>
@@ -6895,7 +6891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>27</v>
       </c>
@@ -6912,7 +6908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>29</v>
       </c>
@@ -6929,7 +6925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>8</v>
       </c>
@@ -6946,7 +6942,7 @@
         <v>4.2799999999999998E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>6</v>
       </c>

</xml_diff>